<commit_message>
Changed id type to uint, added 2 new effects
</commit_message>
<xml_diff>
--- a/Assets/Resources/Configurations/NewCards.xlsx
+++ b/Assets/Resources/Configurations/NewCards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\VTuberSim\Assets\Resources\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB83BC2-AA7E-4CE3-B064-38C44928A257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C64CFA-BECC-4062-972A-84F6B5A42CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="1820" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{511D819F-C477-4292-83B8-A2D3252CC88D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{511D819F-C477-4292-83B8-A2D3252CC88D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -646,7 +646,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L6" sqref="A6:L6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84EBBB0-3A7B-46C2-A26E-3E8A62CA3278}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H4" sqref="B3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,7 @@
         <v>51</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I5" t="s">
         <v>57</v>
@@ -1209,7 +1209,7 @@
         <v>59</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1249,7 +1249,7 @@
         <v>65</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1269,7 +1269,7 @@
         <v>65</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1289,7 +1289,7 @@
         <v>65</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -1309,7 +1309,7 @@
         <v>70</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
         <v>75</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I12" t="s">
         <v>78</v>
@@ -1343,7 +1343,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="A19:B21"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37E88A6-8C6F-4D79-A09C-50AB8814C23D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,5 +1518,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added buff latency, modified attribute modification logic, added 2 buffs
</commit_message>
<xml_diff>
--- a/Assets/Resources/Configurations/NewCards.xlsx
+++ b/Assets/Resources/Configurations/NewCards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\VTuberSim\Assets\Resources\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C64CFA-BECC-4062-972A-84F6B5A42CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2417F30-E793-46A9-89D8-C7BAC18433D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{511D819F-C477-4292-83B8-A2D3252CC88D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -222,12 +222,6 @@
     <t>Reduce Stamina Cost by 2 Points</t>
   </si>
   <si>
-    <t>VStaminaCostModiferEffect</t>
-  </si>
-  <si>
-    <t>OnPreCardApply</t>
-  </si>
-  <si>
     <t>AddBuff_0</t>
   </si>
   <si>
@@ -288,7 +282,19 @@
     <t>NE2Param</t>
   </si>
   <si>
-    <t>Points</t>
+    <t>Latency</t>
+  </si>
+  <si>
+    <t>E2UpgradedParam</t>
+  </si>
+  <si>
+    <t>E1UpgradedParam</t>
+  </si>
+  <si>
+    <t>VAttributeGainPointsModifierEffect</t>
+  </si>
+  <si>
+    <t>OnTurnBegin</t>
   </si>
 </sst>
 </file>
@@ -643,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963A3D60-24B6-48D4-A264-5BC3C590ED89}">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,17 +668,19 @@
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" customWidth="1"/>
-    <col min="21" max="22" width="12.42578125" customWidth="1"/>
-    <col min="23" max="23" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" customWidth="1"/>
+    <col min="23" max="24" width="12.42578125" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -710,43 +718,49 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -774,8 +788,11 @@
       <c r="L2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -803,8 +820,11 @@
       <c r="L3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -832,8 +852,11 @@
       <c r="L4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -861,8 +884,11 @@
       <c r="L5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -888,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -914,7 +940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -942,8 +968,11 @@
       <c r="L8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -971,8 +1000,11 @@
       <c r="L9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -998,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1026,13 +1058,16 @@
       <c r="L11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
         <v>35</v>
@@ -1053,6 +1088,9 @@
         <v>10</v>
       </c>
       <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
         <v>2</v>
       </c>
     </row>
@@ -1064,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84EBBB0-3A7B-46C2-A26E-3E8A62CA3278}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H4" sqref="B3:H4"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,15 +1113,16 @@
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1099,20 +1138,23 @@
       <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1128,11 +1170,14 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1148,14 +1193,17 @@
       <c r="E3" t="s">
         <v>52</v>
       </c>
-      <c r="H3">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1168,14 +1216,17 @@
       <c r="D4" t="s">
         <v>51</v>
       </c>
-      <c r="H4">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1188,14 +1239,17 @@
       <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="H5">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>-1</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1208,11 +1262,14 @@
       <c r="D6" t="s">
         <v>59</v>
       </c>
-      <c r="H6">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1223,113 +1280,131 @@
         <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>-1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
         <v>63</v>
       </c>
-      <c r="C8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>-1</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9">
+        <v>63</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>-1</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10">
+        <v>63</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>-1</v>
       </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11">
+        <v>68</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12">
+        <v>73</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>-1</v>
       </c>
-      <c r="I12" t="s">
-        <v>78</v>
+      <c r="J12" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1343,7 +1418,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,10 +1472,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1417,10 +1492,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1437,16 +1512,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1490,7 +1565,7 @@
         <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Added PickCard Button, Changed persistent buff logic
</commit_message>
<xml_diff>
--- a/Assets/Resources/Configurations/NewCards.xlsx
+++ b/Assets/Resources/Configurations/NewCards.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\VTuberSim\Assets\Resources\Configurations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E1E356-B2A8-47A7-80F6-14DF58C5EE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="10480"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -21,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="138">
   <si>
     <t>ID</t>
   </si>
@@ -438,366 +442,36 @@
   </si>
   <si>
     <t>BAStamina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">再一次 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">下一张使用的牌会使用两次 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -823,318 +497,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1392,47 +777,46 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AA18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.41666666666667" customWidth="1"/>
-    <col min="2" max="2" width="8.75" customWidth="1"/>
-    <col min="3" max="3" width="38.2833333333333" customWidth="1"/>
-    <col min="4" max="4" width="10.425" customWidth="1"/>
-    <col min="5" max="5" width="13.425" customWidth="1"/>
-    <col min="6" max="6" width="10.5666666666667" customWidth="1"/>
-    <col min="7" max="7" width="14.425" customWidth="1"/>
-    <col min="8" max="8" width="7.14166666666667" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="38.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" style="2" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.2833333333333" customWidth="1"/>
-    <col min="11" max="11" width="13.6666666666667" customWidth="1"/>
-    <col min="12" max="12" width="9.70833333333333" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.1416666666667" style="5" customWidth="1"/>
-    <col min="14" max="14" width="17.7083333333333" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" customWidth="1"/>
+    <col min="14" max="14" width="17.7265625" style="3" customWidth="1"/>
     <col min="15" max="15" width="11" style="2" customWidth="1"/>
-    <col min="16" max="16" width="12.2833333333333" customWidth="1"/>
-    <col min="17" max="17" width="17.1416666666667" style="3" customWidth="1"/>
+    <col min="16" max="16" width="12.26953125" customWidth="1"/>
+    <col min="17" max="17" width="17.1796875" style="3" customWidth="1"/>
     <col min="18" max="18" width="9" style="2"/>
-    <col min="20" max="20" width="17.7083333333333" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.7083333333333" style="2" customWidth="1"/>
+    <col min="20" max="20" width="17.7265625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="10.7265625" style="2" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="17.7083333333333" style="3" customWidth="1"/>
-    <col min="24" max="24" width="12.425" style="2" customWidth="1"/>
-    <col min="25" max="25" width="12.425" style="3" customWidth="1"/>
-    <col min="26" max="26" width="12.2833333333333" customWidth="1"/>
+    <col min="23" max="23" width="17.7265625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="12.453125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="12.453125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -1469,13 +853,13 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -1518,7 +902,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:27">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1546,17 +930,17 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="2">
         <v>11</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2">
         <v>7</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:27">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1584,17 +968,17 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" s="4">
-        <v>2</v>
-      </c>
-      <c r="M3" s="5">
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3">
         <v>4</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:27">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1622,17 +1006,17 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="2">
         <v>11</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4">
         <v>15</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:27">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1660,13 +1044,13 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="2">
         <v>11</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5">
         <v>5</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="3">
         <v>5</v>
       </c>
       <c r="O5" s="2">
@@ -1679,7 +1063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:27">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1710,11 +1094,11 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1742,11 +1126,11 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:27">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1777,13 +1161,13 @@
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="L8" s="4">
-        <v>2</v>
-      </c>
-      <c r="M8" s="5">
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8">
         <v>7</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="3">
         <v>7</v>
       </c>
       <c r="O8" s="2">
@@ -1805,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:27">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1833,13 +1217,13 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="2">
         <v>17</v>
       </c>
-      <c r="M9" s="5">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
         <v>1</v>
       </c>
       <c r="O9" s="2">
@@ -1852,7 +1236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:27">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1880,13 +1264,13 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="2">
         <v>6</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10">
         <v>3</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="3">
         <v>4</v>
       </c>
       <c r="O10" s="2">
@@ -1899,7 +1283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:27">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1927,13 +1311,13 @@
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="2">
         <v>7</v>
       </c>
-      <c r="M11" s="5">
-        <v>2</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11" s="3">
         <v>3</v>
       </c>
       <c r="O11" s="2">
@@ -1946,7 +1330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:27">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1974,13 +1358,13 @@
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="2">
         <v>15</v>
       </c>
-      <c r="M12" s="5">
-        <v>2</v>
-      </c>
-      <c r="N12" s="6">
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3">
         <v>3</v>
       </c>
       <c r="O12" s="2">
@@ -1993,7 +1377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:27">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2021,13 +1405,13 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="2">
         <v>11</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13">
         <v>9</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="3">
         <v>13</v>
       </c>
       <c r="O13" s="2">
@@ -2040,7 +1424,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:27">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2068,13 +1452,13 @@
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="2">
         <v>11</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14">
         <v>11</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="3">
         <v>15</v>
       </c>
       <c r="O14" s="2">
@@ -2087,7 +1471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:27">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2115,17 +1499,17 @@
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="2">
         <v>6</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15">
         <v>6</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:27">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2153,17 +1537,17 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="2">
         <v>18</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16">
         <v>1.4</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="3">
         <v>1.8</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2191,13 +1575,13 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="2">
         <v>6</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17">
         <v>4</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="3">
         <v>5</v>
       </c>
       <c r="O17" s="2">
@@ -2207,7 +1591,7 @@
         <v>0.8</v>
       </c>
       <c r="Q17" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -2238,13 +1622,13 @@
       <c r="K18">
         <v>1</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="2">
         <v>19</v>
       </c>
-      <c r="M18" s="5">
-        <v>1</v>
-      </c>
-      <c r="N18" s="6">
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3">
         <v>1</v>
       </c>
       <c r="O18" s="2">
@@ -2266,34 +1650,63 @@
         <v>4</v>
       </c>
     </row>
+    <row r="19" spans="1:20">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="2">
+        <v>6</v>
+      </c>
+      <c r="I19" s="3">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="$A20:$XFD20"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.425" customWidth="1"/>
-    <col min="2" max="2" width="21.1416666666667" customWidth="1"/>
+    <col min="1" max="1" width="3.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="19.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="8" width="10.2833333333333" customWidth="1"/>
-    <col min="9" max="9" width="15.1416666666667" customWidth="1"/>
+    <col min="7" max="8" width="10.26953125" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2831,31 +2244,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.425" customWidth="1"/>
-    <col min="2" max="2" width="23.1416666666667" customWidth="1"/>
-    <col min="3" max="3" width="14.425" customWidth="1"/>
-    <col min="4" max="5" width="16.1416666666667" customWidth="1"/>
-    <col min="6" max="6" width="12.425" customWidth="1"/>
-    <col min="7" max="7" width="14.425" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="5" width="16.1796875" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="10.1416666666667" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2894,7 +2305,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2923,7 +2334,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2946,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2969,7 +2380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2992,7 +2403,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3015,7 +2426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3040,27 +2451,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="4.85833333333333" customWidth="1"/>
-    <col min="2" max="2" width="22.7083333333333" customWidth="1"/>
-    <col min="3" max="3" width="20.1416666666667" customWidth="1"/>
-    <col min="4" max="4" width="15.5666666666667" customWidth="1"/>
-    <col min="5" max="5" width="16.1416666666667" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3087,7 +2496,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3106,7 +2515,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Stamina not changing
</commit_message>
<xml_diff>
--- a/Assets/Resources/Configurations/NewCards.xlsx
+++ b/Assets/Resources/Configurations/NewCards.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\VTuberSim\Assets\Resources\Configurations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2392329D-5653-4239-8B07-65461FB2BB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="10480" activeTab="3"/>
+    <workbookView xWindow="25490" yWindow="1820" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -21,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -527,361 +531,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -907,318 +575,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1476,47 +855,46 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="N29" sqref="C27 N29"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.41666666666667" customWidth="1"/>
-    <col min="2" max="2" width="8.75" customWidth="1"/>
-    <col min="3" max="3" width="44.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="10.425" customWidth="1"/>
-    <col min="5" max="5" width="13.425" customWidth="1"/>
-    <col min="6" max="6" width="10.5666666666667" customWidth="1"/>
-    <col min="7" max="7" width="14.425" customWidth="1"/>
-    <col min="8" max="8" width="7.14166666666667" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.2833333333333" customWidth="1"/>
-    <col min="11" max="11" width="13.6666666666667" customWidth="1"/>
-    <col min="12" max="12" width="9.70833333333333" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.1416666666667" style="5" customWidth="1"/>
-    <col min="14" max="14" width="17.7083333333333" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="3" customWidth="1"/>
     <col min="15" max="15" width="11" style="2" customWidth="1"/>
-    <col min="16" max="16" width="12.2833333333333" customWidth="1"/>
-    <col min="17" max="17" width="17.1416666666667" style="3" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" style="3" customWidth="1"/>
     <col min="18" max="18" width="9" style="2"/>
-    <col min="20" max="20" width="17.7083333333333" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.7083333333333" style="2" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" style="3" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="2" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="17.7083333333333" style="3" customWidth="1"/>
-    <col min="24" max="24" width="12.425" style="2" customWidth="1"/>
-    <col min="25" max="25" width="12.425" style="3" customWidth="1"/>
-    <col min="26" max="26" width="12.2833333333333" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -1553,13 +931,13 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -1602,7 +980,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:27">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1633,17 +1011,17 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="2">
         <v>11</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2">
         <v>7</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:27">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1674,17 +1052,17 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" s="4">
-        <v>2</v>
-      </c>
-      <c r="M3" s="5">
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3">
         <v>4</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:27">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1715,17 +1093,17 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="2">
         <v>11</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4">
         <v>15</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:27">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1756,13 +1134,13 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="2">
         <v>11</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5">
         <v>5</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="3">
         <v>5</v>
       </c>
       <c r="O5" s="2">
@@ -1775,7 +1153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:27">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1809,11 +1187,11 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1844,11 +1222,11 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:27">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1882,13 +1260,13 @@
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="L8" s="4">
-        <v>2</v>
-      </c>
-      <c r="M8" s="5">
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8">
         <v>7</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="3">
         <v>7</v>
       </c>
       <c r="O8" s="2">
@@ -1910,7 +1288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:27">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1941,13 +1319,13 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="2">
         <v>17</v>
       </c>
-      <c r="M9" s="5">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
         <v>1</v>
       </c>
       <c r="O9" s="2">
@@ -1960,7 +1338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:27">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1991,13 +1369,13 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="2">
         <v>6</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10">
         <v>3</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="3">
         <v>4</v>
       </c>
       <c r="O10" s="2">
@@ -2010,7 +1388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:27">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2041,13 +1419,13 @@
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="2">
         <v>7</v>
       </c>
-      <c r="M11" s="5">
-        <v>2</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11" s="3">
         <v>3</v>
       </c>
       <c r="O11" s="2">
@@ -2060,7 +1438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:27">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2091,13 +1469,13 @@
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="2">
         <v>15</v>
       </c>
-      <c r="M12" s="5">
-        <v>2</v>
-      </c>
-      <c r="N12" s="6">
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3">
         <v>3</v>
       </c>
       <c r="O12" s="2">
@@ -2110,7 +1488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:27">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2141,13 +1519,13 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="2">
         <v>11</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13">
         <v>9</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="3">
         <v>13</v>
       </c>
       <c r="O13" s="2">
@@ -2160,7 +1538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:27">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2191,13 +1569,13 @@
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="2">
         <v>11</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14">
         <v>11</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="3">
         <v>15</v>
       </c>
       <c r="O14" s="2">
@@ -2210,7 +1588,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:27">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2241,17 +1619,17 @@
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="2">
         <v>6</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15">
         <v>6</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:27">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2282,17 +1660,17 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="2">
         <v>18</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16">
         <v>1.4</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="3">
         <v>1.8</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2323,13 +1701,13 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="2">
         <v>6</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17">
         <v>4</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="3">
         <v>5</v>
       </c>
       <c r="O17" s="2">
@@ -2339,7 +1717,7 @@
         <v>0.8</v>
       </c>
       <c r="Q17" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -2373,13 +1751,13 @@
       <c r="K18">
         <v>1</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="2">
         <v>19</v>
       </c>
-      <c r="M18" s="5">
-        <v>1</v>
-      </c>
-      <c r="N18" s="6">
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3">
         <v>1</v>
       </c>
       <c r="O18" s="2">
@@ -2401,7 +1779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2432,11 +1810,11 @@
       <c r="K19">
         <v>1</v>
       </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2467,17 +1845,17 @@
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="2">
         <v>15</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20">
         <v>5</v>
       </c>
-      <c r="N20" s="6">
+      <c r="N20" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:20">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2508,16 +1886,16 @@
       <c r="K21">
         <v>1</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="2">
         <v>23</v>
       </c>
-      <c r="M21" s="5">
-        <v>1</v>
-      </c>
-      <c r="N21" s="6">
-        <v>1</v>
-      </c>
-      <c r="O21" s="4">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2">
         <v>7</v>
       </c>
       <c r="P21">
@@ -2527,7 +1905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2558,13 +1936,13 @@
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="2">
         <v>24</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22">
         <v>24</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="3">
         <v>30</v>
       </c>
     </row>
@@ -2658,13 +2036,13 @@
       <c r="K24">
         <v>1</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="2">
         <v>26</v>
       </c>
-      <c r="M24" s="5">
-        <v>2</v>
-      </c>
-      <c r="N24" s="6">
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24" s="3">
         <v>2</v>
       </c>
       <c r="O24" s="2">
@@ -2686,7 +2064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:20">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2717,13 +2095,13 @@
       <c r="K25">
         <v>1</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="2">
         <v>6</v>
       </c>
-      <c r="M25" s="5">
-        <v>2</v>
-      </c>
-      <c r="N25" s="6">
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25" s="3">
         <v>4</v>
       </c>
       <c r="O25" s="2">
@@ -2738,32 +2116,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="$A29:$XFD29"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.425" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="19.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="8" width="10.2833333333333" customWidth="1"/>
-    <col min="9" max="9" width="15.1416666666667" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2832,7 +2207,6 @@
       <c r="F3" t="s">
         <v>92</v>
       </c>
-      <c r="G3"/>
       <c r="I3">
         <v>1</v>
       </c>
@@ -3050,7 +2424,6 @@
       <c r="F14" t="s">
         <v>92</v>
       </c>
-      <c r="G14"/>
       <c r="I14">
         <v>-1</v>
       </c>
@@ -3235,7 +2608,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" customFormat="1" spans="1:9">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3254,7 +2627,6 @@
       <c r="F24" t="s">
         <v>92</v>
       </c>
-      <c r="G24"/>
       <c r="I24">
         <v>-1</v>
       </c>
@@ -3322,7 +2694,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" customFormat="1" spans="1:9">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3356,7 +2728,7 @@
         <v>106</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" t="s">
         <v>139</v>
@@ -3390,31 +2762,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.425" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="14.425" customWidth="1"/>
-    <col min="4" max="5" width="16.1416666666667" customWidth="1"/>
-    <col min="6" max="6" width="12.425" customWidth="1"/>
-    <col min="7" max="7" width="14.425" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="10.1416666666667" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3453,7 +2823,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3482,7 +2852,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3505,7 +2875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3528,7 +2898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3551,7 +2921,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3574,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3597,7 +2967,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3620,7 +2990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3643,7 +3013,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3668,29 +3038,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D8" sqref="D2 D3 D8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.85833333333333" customWidth="1"/>
-    <col min="2" max="2" width="22.7083333333333" customWidth="1"/>
-    <col min="3" max="3" width="20.1416666666667" customWidth="1"/>
-    <col min="4" max="4" width="15.5666666666667" customWidth="1"/>
-    <col min="5" max="5" width="16.1416666666667" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="11.0916666666667" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3716,7 +3084,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3736,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3749,13 +3117,12 @@
       <c r="D3" t="s">
         <v>161</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Turn Begin Buff Apply Logic
</commit_message>
<xml_diff>
--- a/Assets/Resources/Configurations/NewCards.xlsx
+++ b/Assets/Resources/Configurations/NewCards.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\VTuberSim\Assets\Resources\Configurations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB0A762-4BD8-435E-B398-DF6A00A0D8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="10480"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -21,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -557,361 +561,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -937,318 +605,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1506,47 +885,46 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29:G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.41666666666667" customWidth="1"/>
-    <col min="2" max="2" width="8.75" customWidth="1"/>
-    <col min="3" max="3" width="44.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="10.425" customWidth="1"/>
-    <col min="5" max="5" width="13.425" customWidth="1"/>
-    <col min="6" max="6" width="10.5666666666667" customWidth="1"/>
-    <col min="7" max="7" width="9.66666666666667" customWidth="1"/>
-    <col min="8" max="8" width="7.14166666666667" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.2833333333333" customWidth="1"/>
-    <col min="11" max="11" width="13.6666666666667" customWidth="1"/>
-    <col min="12" max="12" width="9.70833333333333" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.1416666666667" style="5" customWidth="1"/>
-    <col min="14" max="14" width="17.7083333333333" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="3" customWidth="1"/>
     <col min="15" max="15" width="11" style="2" customWidth="1"/>
-    <col min="16" max="16" width="12.2833333333333" customWidth="1"/>
-    <col min="17" max="17" width="17.1416666666667" style="3" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" style="3" customWidth="1"/>
     <col min="18" max="18" width="9" style="2"/>
-    <col min="20" max="20" width="17.7083333333333" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.7083333333333" style="2" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" style="3" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="2" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="17.7083333333333" style="3" customWidth="1"/>
-    <col min="24" max="24" width="12.425" style="2" customWidth="1"/>
-    <col min="25" max="25" width="12.425" style="3" customWidth="1"/>
-    <col min="26" max="26" width="12.2833333333333" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -1583,13 +961,13 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -1632,7 +1010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:27">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1663,17 +1041,17 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="2">
         <v>11</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2">
         <v>7</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:27">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1704,17 +1082,17 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" s="4">
-        <v>2</v>
-      </c>
-      <c r="M3" s="5">
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3">
         <v>4</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:27">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1745,17 +1123,17 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="2">
         <v>11</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4">
         <v>15</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:27">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1786,13 +1164,13 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="2">
         <v>11</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5">
         <v>5</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="3">
         <v>5</v>
       </c>
       <c r="O5" s="2">
@@ -1805,7 +1183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:27">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1839,11 +1217,11 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1874,11 +1252,11 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:27">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1912,13 +1290,13 @@
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="L8" s="4">
-        <v>2</v>
-      </c>
-      <c r="M8" s="5">
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8">
         <v>7</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="3">
         <v>7</v>
       </c>
       <c r="O8" s="2">
@@ -1940,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:27">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1971,13 +1349,13 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="2">
         <v>17</v>
       </c>
-      <c r="M9" s="5">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
         <v>1</v>
       </c>
       <c r="O9" s="2">
@@ -1990,7 +1368,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:27">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2021,13 +1399,13 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="2">
         <v>6</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10">
         <v>3</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="3">
         <v>4</v>
       </c>
       <c r="O10" s="2">
@@ -2040,7 +1418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:27">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2071,13 +1449,13 @@
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="2">
         <v>7</v>
       </c>
-      <c r="M11" s="5">
-        <v>2</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11" s="3">
         <v>3</v>
       </c>
       <c r="O11" s="2">
@@ -2090,7 +1468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:27">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2121,13 +1499,13 @@
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="2">
         <v>15</v>
       </c>
-      <c r="M12" s="5">
-        <v>2</v>
-      </c>
-      <c r="N12" s="6">
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3">
         <v>3</v>
       </c>
       <c r="O12" s="2">
@@ -2140,7 +1518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:27">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2171,13 +1549,13 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="2">
         <v>11</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13">
         <v>9</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="3">
         <v>13</v>
       </c>
       <c r="O13" s="2">
@@ -2190,7 +1568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:27">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2221,13 +1599,13 @@
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="2">
         <v>11</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14">
         <v>11</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="3">
         <v>15</v>
       </c>
       <c r="O14" s="2">
@@ -2240,7 +1618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:27">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2271,17 +1649,17 @@
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="2">
         <v>6</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15">
         <v>6</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:27">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2312,17 +1690,17 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="2">
         <v>18</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16">
         <v>1.4</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="3">
         <v>1.8</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2353,13 +1731,13 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="2">
         <v>6</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17">
         <v>4</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="3">
         <v>5</v>
       </c>
       <c r="O17" s="2">
@@ -2369,7 +1747,7 @@
         <v>0.8</v>
       </c>
       <c r="Q17" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -2403,13 +1781,13 @@
       <c r="K18">
         <v>1</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="2">
         <v>19</v>
       </c>
-      <c r="M18" s="5">
-        <v>1</v>
-      </c>
-      <c r="N18" s="6">
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3">
         <v>1</v>
       </c>
       <c r="O18" s="2">
@@ -2431,7 +1809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2462,11 +1840,11 @@
       <c r="K19">
         <v>1</v>
       </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2497,17 +1875,17 @@
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="2">
         <v>15</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20">
         <v>5</v>
       </c>
-      <c r="N20" s="6">
+      <c r="N20" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:20">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2538,16 +1916,16 @@
       <c r="K21">
         <v>1</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="2">
         <v>23</v>
       </c>
-      <c r="M21" s="5">
-        <v>1</v>
-      </c>
-      <c r="N21" s="6">
-        <v>1</v>
-      </c>
-      <c r="O21" s="4">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2">
         <v>7</v>
       </c>
       <c r="P21">
@@ -2557,7 +1935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2588,13 +1966,13 @@
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="2">
         <v>24</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22">
         <v>24</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="3">
         <v>30</v>
       </c>
     </row>
@@ -2688,13 +2066,13 @@
       <c r="K24">
         <v>1</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="2">
         <v>26</v>
       </c>
-      <c r="M24" s="5">
-        <v>2</v>
-      </c>
-      <c r="N24" s="6">
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24" s="3">
         <v>2</v>
       </c>
       <c r="O24" s="2">
@@ -2716,7 +2094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:20">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2747,13 +2125,13 @@
       <c r="K25">
         <v>1</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="2">
         <v>6</v>
       </c>
-      <c r="M25" s="5">
-        <v>2</v>
-      </c>
-      <c r="N25" s="6">
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25" s="3">
         <v>4</v>
       </c>
       <c r="O25" s="2">
@@ -2766,7 +2144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:20">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2797,13 +2175,13 @@
       <c r="K26">
         <v>0</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="2">
         <v>6</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26">
         <v>5</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N26" s="3">
         <v>7</v>
       </c>
       <c r="O26" s="2">
@@ -2816,7 +2194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:20">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2847,13 +2225,13 @@
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="2">
         <v>15</v>
       </c>
-      <c r="M27" s="5">
+      <c r="M27">
         <v>3</v>
       </c>
-      <c r="N27" s="6">
+      <c r="N27" s="3">
         <v>4</v>
       </c>
       <c r="O27" s="2">
@@ -2866,7 +2244,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:20">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2897,17 +2275,17 @@
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="2">
         <v>7</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28">
         <v>3</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N28" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:20">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2938,13 +2316,13 @@
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="2">
         <v>7</v>
       </c>
-      <c r="M29" s="5">
+      <c r="M29">
         <v>3</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29" s="3">
         <v>4</v>
       </c>
       <c r="O29" s="2">
@@ -2991,13 +2369,13 @@
       <c r="K30">
         <v>1</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="2">
         <v>15</v>
       </c>
-      <c r="M30" s="5">
+      <c r="M30">
         <v>3</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30" s="3">
         <v>4</v>
       </c>
       <c r="O30" s="2">
@@ -3021,32 +2399,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="$A31:$XFD31"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.425" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="19.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="8" width="10.2833333333333" customWidth="1"/>
-    <col min="9" max="9" width="15.1416666666667" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3516,7 +2891,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" customFormat="1" spans="1:9">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3535,7 +2910,6 @@
       <c r="F24" t="s">
         <v>102</v>
       </c>
-      <c r="G24"/>
       <c r="I24">
         <v>-1</v>
       </c>
@@ -3603,7 +2977,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" customFormat="1" spans="1:9">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3671,31 +3045,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A11:G12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.425" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="14.425" customWidth="1"/>
-    <col min="4" max="5" width="16.1416666666667" customWidth="1"/>
-    <col min="6" max="6" width="12.425" customWidth="1"/>
-    <col min="7" max="7" width="14.425" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="10.1416666666667" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3734,7 +3106,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3763,7 +3135,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3786,7 +3158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3809,7 +3181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3832,7 +3204,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3855,7 +3227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3878,7 +3250,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3901,7 +3273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3924,7 +3296,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3949,29 +3321,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D8" sqref="D2 D3 D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.85833333333333" customWidth="1"/>
-    <col min="2" max="2" width="22.7083333333333" customWidth="1"/>
-    <col min="3" max="3" width="20.1416666666667" customWidth="1"/>
-    <col min="4" max="4" width="15.5666666666667" customWidth="1"/>
-    <col min="5" max="5" width="16.1416666666667" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="11.0916666666667" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3997,7 +3367,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4017,7 +3387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4036,7 +3406,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Buff Latency Logic
</commit_message>
<xml_diff>
--- a/Assets/Resources/Configurations/NewCards.xlsx
+++ b/Assets/Resources/Configurations/NewCards.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\VTuberSim\Assets\Resources\Configurations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880D011E-E76C-46B3-A412-BEB0B354738A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="10480"/>
+    <workbookView xWindow="25490" yWindow="1820" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -21,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -614,361 +618,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -994,318 +662,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1563,47 +942,46 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.41666666666667" customWidth="1"/>
-    <col min="2" max="2" width="8.75" customWidth="1"/>
-    <col min="3" max="3" width="44.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="10.425" customWidth="1"/>
-    <col min="5" max="5" width="13.425" customWidth="1"/>
-    <col min="6" max="6" width="10.5666666666667" customWidth="1"/>
-    <col min="7" max="7" width="9.66666666666667" customWidth="1"/>
-    <col min="8" max="8" width="7.14166666666667" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.2833333333333" customWidth="1"/>
-    <col min="11" max="11" width="13.6666666666667" customWidth="1"/>
-    <col min="12" max="12" width="9.70833333333333" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.1416666666667" style="5" customWidth="1"/>
-    <col min="14" max="14" width="17.7083333333333" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="3" customWidth="1"/>
     <col min="15" max="15" width="11" style="2" customWidth="1"/>
-    <col min="16" max="16" width="12.2833333333333" customWidth="1"/>
-    <col min="17" max="17" width="17.1416666666667" style="3" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" style="3" customWidth="1"/>
     <col min="18" max="18" width="9" style="2"/>
-    <col min="20" max="20" width="17.7083333333333" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.7083333333333" style="2" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" style="3" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="2" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="17.7083333333333" style="3" customWidth="1"/>
-    <col min="24" max="24" width="12.425" style="2" customWidth="1"/>
-    <col min="25" max="25" width="12.425" style="3" customWidth="1"/>
-    <col min="26" max="26" width="12.2833333333333" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -1640,13 +1018,13 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -1689,7 +1067,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:27">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1720,17 +1098,17 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="2">
         <v>11</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2">
         <v>7</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:27">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1761,17 +1139,17 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" s="4">
-        <v>2</v>
-      </c>
-      <c r="M3" s="5">
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3">
         <v>4</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:27">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1802,17 +1180,17 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="2">
         <v>11</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4">
         <v>15</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:27">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1843,13 +1221,13 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="2">
         <v>11</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5">
         <v>5</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="3">
         <v>5</v>
       </c>
       <c r="O5" s="2">
@@ -1862,7 +1240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:27">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1896,11 +1274,11 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1931,11 +1309,11 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:27">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1969,13 +1347,13 @@
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="L8" s="4">
-        <v>2</v>
-      </c>
-      <c r="M8" s="5">
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8">
         <v>7</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="3">
         <v>7</v>
       </c>
       <c r="O8" s="2">
@@ -1997,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:27">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2028,13 +1406,13 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="2">
         <v>17</v>
       </c>
-      <c r="M9" s="5">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
         <v>1</v>
       </c>
       <c r="O9" s="2">
@@ -2047,7 +1425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:27">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2078,13 +1456,13 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="2">
         <v>6</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10">
         <v>3</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="3">
         <v>4</v>
       </c>
       <c r="O10" s="2">
@@ -2097,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:27">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2128,13 +1506,13 @@
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="2">
         <v>7</v>
       </c>
-      <c r="M11" s="5">
-        <v>2</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11" s="3">
         <v>3</v>
       </c>
       <c r="O11" s="2">
@@ -2147,7 +1525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:27">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2178,13 +1556,13 @@
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="2">
         <v>15</v>
       </c>
-      <c r="M12" s="5">
-        <v>2</v>
-      </c>
-      <c r="N12" s="6">
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3">
         <v>3</v>
       </c>
       <c r="O12" s="2">
@@ -2197,7 +1575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:27">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2228,13 +1606,13 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="2">
         <v>11</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13">
         <v>9</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="3">
         <v>13</v>
       </c>
       <c r="O13" s="2">
@@ -2247,7 +1625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:27">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2278,13 +1656,13 @@
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="2">
         <v>11</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14">
         <v>11</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="3">
         <v>15</v>
       </c>
       <c r="O14" s="2">
@@ -2297,7 +1675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:27">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2328,17 +1706,17 @@
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="2">
         <v>6</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15">
         <v>6</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:27">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2369,17 +1747,17 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="2">
         <v>18</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16">
         <v>1.4</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="3">
         <v>1.8</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2410,13 +1788,13 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="2">
         <v>6</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17">
         <v>4</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="3">
         <v>5</v>
       </c>
       <c r="O17" s="2">
@@ -2426,7 +1804,7 @@
         <v>0.8</v>
       </c>
       <c r="Q17" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -2460,13 +1838,13 @@
       <c r="K18">
         <v>1</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="2">
         <v>19</v>
       </c>
-      <c r="M18" s="5">
-        <v>1</v>
-      </c>
-      <c r="N18" s="6">
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3">
         <v>1</v>
       </c>
       <c r="O18" s="2">
@@ -2488,7 +1866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2519,11 +1897,11 @@
       <c r="K19">
         <v>1</v>
       </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2554,17 +1932,17 @@
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="2">
         <v>15</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20">
         <v>5</v>
       </c>
-      <c r="N20" s="6">
+      <c r="N20" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:20">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2595,16 +1973,16 @@
       <c r="K21">
         <v>1</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="2">
         <v>23</v>
       </c>
-      <c r="M21" s="5">
-        <v>1</v>
-      </c>
-      <c r="N21" s="6">
-        <v>1</v>
-      </c>
-      <c r="O21" s="4">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2">
         <v>7</v>
       </c>
       <c r="P21">
@@ -2614,7 +1992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2645,13 +2023,13 @@
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="2">
         <v>24</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22">
         <v>24</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="3">
         <v>30</v>
       </c>
     </row>
@@ -2745,13 +2123,13 @@
       <c r="K24">
         <v>1</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="2">
         <v>26</v>
       </c>
-      <c r="M24" s="5">
-        <v>2</v>
-      </c>
-      <c r="N24" s="6">
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24" s="3">
         <v>2</v>
       </c>
       <c r="O24" s="2">
@@ -2773,7 +2151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:20">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2804,13 +2182,13 @@
       <c r="K25">
         <v>1</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="2">
         <v>6</v>
       </c>
-      <c r="M25" s="5">
-        <v>2</v>
-      </c>
-      <c r="N25" s="6">
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25" s="3">
         <v>4</v>
       </c>
       <c r="O25" s="2">
@@ -2823,7 +2201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:20">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2854,13 +2232,13 @@
       <c r="K26">
         <v>0</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="2">
         <v>6</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26">
         <v>5</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N26" s="3">
         <v>7</v>
       </c>
       <c r="O26" s="2">
@@ -2873,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:20">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2904,13 +2282,13 @@
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="2">
         <v>15</v>
       </c>
-      <c r="M27" s="5">
+      <c r="M27">
         <v>3</v>
       </c>
-      <c r="N27" s="6">
+      <c r="N27" s="3">
         <v>4</v>
       </c>
       <c r="O27" s="2">
@@ -2923,7 +2301,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:20">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2954,17 +2332,17 @@
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="2">
         <v>7</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28">
         <v>3</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N28" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:20">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2995,13 +2373,13 @@
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="2">
         <v>7</v>
       </c>
-      <c r="M29" s="5">
+      <c r="M29">
         <v>3</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29" s="3">
         <v>4</v>
       </c>
       <c r="O29" s="2">
@@ -3048,13 +2426,13 @@
       <c r="K30">
         <v>1</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="2">
         <v>15</v>
       </c>
-      <c r="M30" s="5">
+      <c r="M30">
         <v>3</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30" s="3">
         <v>4</v>
       </c>
       <c r="O30" s="2">
@@ -3076,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:20">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3110,13 +2488,13 @@
       <c r="K31">
         <v>1</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31" s="2">
         <v>7</v>
       </c>
-      <c r="M31" s="5">
+      <c r="M31">
         <v>4</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="3">
         <v>6</v>
       </c>
       <c r="O31" s="2">
@@ -3160,13 +2538,13 @@
       <c r="K32">
         <v>1</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32" s="2">
         <v>15</v>
       </c>
-      <c r="M32" s="5">
+      <c r="M32">
         <v>5</v>
       </c>
-      <c r="N32" s="6">
+      <c r="N32" s="3">
         <v>7</v>
       </c>
       <c r="O32" s="2">
@@ -3188,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:20">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3219,13 +2597,13 @@
       <c r="K33">
         <v>0</v>
       </c>
-      <c r="L33" s="4">
-        <v>2</v>
-      </c>
-      <c r="M33" s="5">
+      <c r="L33" s="2">
+        <v>2</v>
+      </c>
+      <c r="M33">
         <v>6</v>
       </c>
-      <c r="N33" s="6">
+      <c r="N33" s="3">
         <v>8</v>
       </c>
     </row>
@@ -3260,13 +2638,13 @@
       <c r="K34">
         <v>1</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34" s="2">
         <v>19</v>
       </c>
-      <c r="M34" s="5">
-        <v>1</v>
-      </c>
-      <c r="N34" s="6">
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34" s="3">
         <v>1</v>
       </c>
       <c r="O34" s="2">
@@ -3319,13 +2697,13 @@
       <c r="K35">
         <v>1</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="2">
         <v>32</v>
       </c>
-      <c r="M35" s="5">
+      <c r="M35">
         <v>30</v>
       </c>
-      <c r="N35" s="6">
+      <c r="N35" s="3">
         <v>30</v>
       </c>
       <c r="O35" s="2">
@@ -3347,7 +2725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:20">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3378,13 +2756,13 @@
       <c r="K36">
         <v>1</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36" s="2">
         <v>33</v>
       </c>
-      <c r="M36" s="5">
+      <c r="M36">
         <v>50</v>
       </c>
-      <c r="N36" s="6">
+      <c r="N36" s="3">
         <v>70</v>
       </c>
       <c r="O36" s="2">
@@ -3399,32 +2777,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.425" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="19.3333333333333" customWidth="1"/>
-    <col min="6" max="6" width="18.9166666666667" customWidth="1"/>
-    <col min="7" max="8" width="10.2833333333333" customWidth="1"/>
-    <col min="9" max="9" width="15.1416666666667" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3894,7 +3269,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" customFormat="1" spans="1:9">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3913,7 +3288,6 @@
       <c r="F24" t="s">
         <v>113</v>
       </c>
-      <c r="G24"/>
       <c r="I24">
         <v>-1</v>
       </c>
@@ -3981,7 +3355,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" customFormat="1" spans="1:9">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4070,7 +3444,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" customFormat="1" spans="1:9">
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4090,7 +3464,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" customFormat="1" spans="1:9">
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4152,31 +3526,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.425" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="14.425" customWidth="1"/>
-    <col min="4" max="5" width="16.1416666666667" customWidth="1"/>
-    <col min="6" max="6" width="12.425" customWidth="1"/>
-    <col min="7" max="7" width="14.425" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="10.1416666666667" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4215,7 +3587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4244,7 +3616,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4267,7 +3639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4290,7 +3662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4313,7 +3685,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4336,7 +3708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4359,7 +3731,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4382,7 +3754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4405,7 +3777,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4428,7 +3800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4442,7 +3814,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>29</v>
@@ -4451,7 +3823,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4465,7 +3837,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <v>29</v>
@@ -4476,29 +3848,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.85833333333333" customWidth="1"/>
-    <col min="2" max="2" width="22.7083333333333" customWidth="1"/>
-    <col min="3" max="3" width="20.1416666666667" customWidth="1"/>
-    <col min="4" max="4" width="15.5666666666667" customWidth="1"/>
-    <col min="5" max="5" width="16.1416666666667" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="11.0916666666667" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4524,7 +3894,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4544,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4563,7 +3933,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>